<commit_message>
Consertando Ts na célula de carga, controlador da altitude sintonizado e calibrações feitas para funcionar no laboratório
Setpoint da altitude está sendo enviado do python
</commit_message>
<xml_diff>
--- a/Calibração/CélulaCarga/CalibrandoCelulaCarga.xlsx
+++ b/Calibração/CélulaCarga/CalibrandoCelulaCarga.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITALO DIAS\Desktop\TCC-Drone\Calibração\CélulaCarga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD89ACE4-0360-4C57-9A10-36CD31CA7A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009894FC-9C62-441B-950C-6B795C707A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{097909A5-12FA-4257-A99D-C2302BCA1918}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{097909A5-12FA-4257-A99D-C2302BCA1918}"/>
   </bookViews>
   <sheets>
     <sheet name="Célula de carga" sheetId="5" r:id="rId1"/>
@@ -287,16 +287,16 @@
                   <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>188</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>230</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>280</c:v>
+                  <c:v>291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>325</c:v>
+                  <c:v>338</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -308,25 +308,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>521</c:v>
+                  <c:v>592</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>442</c:v>
+                  <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>367</c:v>
+                  <c:v>420</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>303</c:v>
+                  <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>289</c:v>
+                  <c:v>314</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>214</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>153</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -383,22 +383,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>151</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>190</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>233</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>281</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>325</c:v>
@@ -413,25 +413,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>515</c:v>
+                  <c:v>601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>437</c:v>
+                  <c:v>523</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>364</c:v>
+                  <c:v>443</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>296</c:v>
+                  <c:v>369</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>292</c:v>
+                  <c:v>318</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>211</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>157</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,22 +491,22 @@
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>193</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>234</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>284</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>327</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -518,25 +518,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>522</c:v>
+                  <c:v>592</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>447</c:v>
+                  <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>366</c:v>
+                  <c:v>420</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>298</c:v>
+                  <c:v>342</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>291</c:v>
+                  <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>217</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>163</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -936,25 +936,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>107</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>186</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>261</c:v>
+                  <c:v>301</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>325</c:v>
+                  <c:v>381</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>339</c:v>
+                  <c:v>407</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>414</c:v>
+                  <c:v>453</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>475</c:v>
+                  <c:v>543</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -975,16 +975,16 @@
                   <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>188</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>230</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>280</c:v>
+                  <c:v>291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>325</c:v>
+                  <c:v>338</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1052,8 +1052,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.14182451783317424"/>
-                  <c:y val="7.9505643305521206E-2"/>
+                  <c:x val="0.18276700713231264"/>
+                  <c:y val="2.6228456035440897E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1093,25 +1093,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>109</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>187</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>260</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>328</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>332</c:v>
+                  <c:v>396</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>413</c:v>
+                  <c:v>421</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>467</c:v>
+                  <c:v>504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1123,22 +1123,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>151</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>190</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>233</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>281</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>325</c:v>
@@ -1209,8 +1209,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.14030689759951381"/>
-                  <c:y val="3.0713096747598399E-2"/>
+                  <c:x val="0.13621975466375727"/>
+                  <c:y val="-3.9449653783336723E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1250,25 +1250,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>109</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>184</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>265</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>333</c:v>
+                  <c:v>372</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>340</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>414</c:v>
+                  <c:v>447</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>468</c:v>
+                  <c:v>536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,22 +1283,22 @@
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>193</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>234</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>284</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>327</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3123,8 +3123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE102C0D-F012-4751-83AF-85358933C2BB}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3141,7 +3141,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="3">
-        <v>628</v>
+        <v>721</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -3150,7 +3150,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="2">
-        <v>624</v>
+        <v>714</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -3159,7 +3159,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="3">
-        <v>631</v>
+        <v>714</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -3202,31 +3202,31 @@
         <v>62</v>
       </c>
       <c r="C3" s="4">
-        <v>521</v>
+        <v>592</v>
       </c>
       <c r="D3" s="4">
         <f>$D$1-C3</f>
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="E3">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F3">
-        <v>515</v>
+        <v>601</v>
       </c>
       <c r="G3">
         <f>$G$1-F3</f>
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H3" s="4">
         <v>63</v>
       </c>
       <c r="I3" s="4">
-        <v>522</v>
+        <v>592</v>
       </c>
       <c r="J3" s="4">
         <f>$J$1-I3</f>
-        <v>109</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -3237,31 +3237,31 @@
         <v>108</v>
       </c>
       <c r="C4" s="4">
-        <v>442</v>
+        <v>505</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" ref="D4:D9" si="0">$D$1-C4</f>
-        <v>186</v>
+        <v>216</v>
       </c>
       <c r="E4">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F4">
-        <v>437</v>
+        <v>523</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G9" si="1">$G$1-F4</f>
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H4" s="4">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I4" s="4">
-        <v>447</v>
+        <v>505</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" ref="J4:J9" si="2">$J$1-I4</f>
-        <v>184</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -3272,31 +3272,31 @@
         <v>150</v>
       </c>
       <c r="C5" s="4">
-        <v>367</v>
+        <v>420</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
-        <v>261</v>
+        <v>301</v>
       </c>
       <c r="E5">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="F5">
-        <v>364</v>
+        <v>443</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="H5" s="4">
         <v>152</v>
       </c>
       <c r="I5" s="4">
-        <v>366</v>
+        <v>420</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" si="2"/>
-        <v>265</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -3304,34 +3304,34 @@
         <v>60</v>
       </c>
       <c r="B6" s="4">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C6" s="4">
-        <v>303</v>
+        <v>340</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>325</v>
+        <v>381</v>
       </c>
       <c r="E6">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="F6">
-        <v>296</v>
+        <v>369</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="H6" s="4">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I6" s="4">
-        <v>298</v>
+        <v>342</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="2"/>
-        <v>333</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -3339,34 +3339,34 @@
         <v>70</v>
       </c>
       <c r="B7" s="4">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="C7" s="4">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>339</v>
+        <v>407</v>
       </c>
       <c r="E7">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="F7">
-        <v>292</v>
+        <v>318</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>332</v>
+        <v>396</v>
       </c>
       <c r="H7" s="4">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="I7" s="4">
-        <v>291</v>
+        <v>321</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="2"/>
-        <v>340</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -3374,34 +3374,34 @@
         <v>80</v>
       </c>
       <c r="B8" s="4">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="C8" s="4">
-        <v>214</v>
+        <v>268</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>414</v>
+        <v>453</v>
       </c>
       <c r="E8">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="F8">
-        <v>211</v>
+        <v>293</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="H8" s="4">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="I8" s="4">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="2"/>
-        <v>414</v>
+        <v>447</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -3409,55 +3409,63 @@
         <v>90</v>
       </c>
       <c r="B9" s="4">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="C9" s="4">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>475</v>
+        <v>543</v>
       </c>
       <c r="E9">
         <v>325</v>
       </c>
       <c r="F9">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>467</v>
+        <v>504</v>
       </c>
       <c r="H9" s="4">
-        <v>327</v>
+        <v>344</v>
       </c>
       <c r="I9" s="4">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="2"/>
-        <v>468</v>
+        <v>536</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>382</v>
+      </c>
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="4">
-        <v>0.64949999999999997</v>
-      </c>
-      <c r="D10" s="4"/>
+        <v>0.58240000000000003</v>
+      </c>
+      <c r="D10" s="4">
+        <v>372</v>
+      </c>
       <c r="E10" t="s">
         <v>19</v>
       </c>
       <c r="F10">
-        <v>0.65749999999999997</v>
+        <v>0.58789999999999998</v>
+      </c>
+      <c r="G10" s="4">
+        <v>385</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="4">
-        <v>0.65790000000000004</v>
+        <v>0.60129999999999995</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" t="s">
@@ -3465,7 +3473,7 @@
       </c>
       <c r="L10" s="5">
         <f>AVERAGE(C10,F10,I10)</f>
-        <v>0.6549666666666667</v>
+        <v>0.59053333333333335</v>
       </c>
       <c r="N10" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Versão final do TCC com comentários
</commit_message>
<xml_diff>
--- a/Calibração/CélulaCarga/CalibrandoCelulaCarga.xlsx
+++ b/Calibração/CélulaCarga/CalibrandoCelulaCarga.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITALO DIAS\Desktop\TCC-Drone\Calibração\CélulaCarga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009894FC-9C62-441B-950C-6B795C707A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C0622C-6BBF-41EB-A799-DA3E4B04BA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{097909A5-12FA-4257-A99D-C2302BCA1918}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{097909A5-12FA-4257-A99D-C2302BCA1918}"/>
   </bookViews>
   <sheets>
     <sheet name="Célula de carga" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Potencia</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>no código precisa dividir por 1000</t>
+  </si>
+  <si>
+    <t>Experimento 1</t>
+  </si>
+  <si>
+    <t>Experimento 3</t>
+  </si>
+  <si>
+    <t>Experimento 2</t>
   </si>
 </sst>
 </file>
@@ -835,7 +844,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.7384910858812453E-2"/>
+          <c:y val="0.117970737913486"/>
+          <c:w val="0.6566903772683409"/>
+          <c:h val="0.74079736931738493"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -848,7 +867,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>exp1</c:v>
+                  <c:v>Experimento 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -895,8 +914,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.12968343633435975"/>
-                  <c:y val="-1.3987205376663901E-2"/>
+                  <c:x val="0.24013950941447343"/>
+                  <c:y val="0.4180912023401655"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1005,7 +1024,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>exp2</c:v>
+                  <c:v>Experimento 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1052,8 +1071,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.18276700713231264"/>
-                  <c:y val="2.6228456035440897E-3"/>
+                  <c:x val="0.28670491634173717"/>
+                  <c:y val="0.48400853519264292"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1162,7 +1181,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>exp3</c:v>
+                  <c:v>Experimento 3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1209,8 +1228,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.13621975466375727"/>
-                  <c:y val="-3.9449653783336723E-2"/>
+                  <c:x val="0.24849738103371974"/>
+                  <c:y val="0.64711486445873656"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1325,6 +1344,8 @@
         <c:axId val="1700330208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="550"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1363,7 +1384,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>Valor na célula de carga - Tara</a:t>
+                  <a:t>Valor lido pelo Arduino - CC</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1437,11 +1458,13 @@
         <c:crossAx val="1700329792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="50"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1700329792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="350"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1565,6 +1588,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.77853975287851929"/>
+          <c:y val="0.17054582156238104"/>
+          <c:w val="0.20560668684471314"/>
+          <c:h val="0.65601370439382101"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2747,16 +2780,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>16057</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>113212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>473257</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>113212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2785,16 +2818,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5444</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>79194</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>61232</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>71574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3123,19 +3156,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE102C0D-F012-4751-83AF-85358933C2BB}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>7</v>
@@ -3143,8 +3176,8 @@
       <c r="D1" s="3">
         <v>721</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -3153,7 +3186,7 @@
         <v>714</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>9</v>
@@ -3162,7 +3195,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3194,7 +3227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>30</v>
       </c>
@@ -3229,7 +3262,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>40</v>
       </c>
@@ -3264,7 +3297,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -3299,7 +3332,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>60</v>
       </c>
@@ -3334,7 +3367,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>70</v>
       </c>
@@ -3369,7 +3402,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>80</v>
       </c>
@@ -3404,7 +3437,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>90</v>
       </c>
@@ -3439,7 +3472,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>382</v>
       </c>
@@ -3479,70 +3512,70 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>

</xml_diff>